<commit_message>
add different kind of data in excel file with right barcodes EAN14
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Штрихкод</t>
   </si>
   <si>
-    <t>2000275733007</t>
-  </si>
-  <si>
     <t>Торговая марка</t>
   </si>
   <si>
@@ -53,75 +50,42 @@
     <t>white</t>
   </si>
   <si>
-    <t>Amour Bridal</t>
-  </si>
-  <si>
     <t>Eva Rossi</t>
   </si>
   <si>
-    <t>Carl Lagerrfield</t>
-  </si>
-  <si>
     <t>Mondi Probucsovich</t>
   </si>
   <si>
     <t>Xfactor</t>
   </si>
   <si>
-    <t>Costa Vog</t>
-  </si>
-  <si>
     <t>Свадебное платье</t>
   </si>
   <si>
     <t>Перчатки-митинки</t>
   </si>
   <si>
-    <t>Детсоке свадебное платье</t>
-  </si>
-  <si>
     <t>Обувь</t>
   </si>
   <si>
-    <t>Туфли</t>
-  </si>
-  <si>
     <t>Босоножки</t>
   </si>
   <si>
     <t>Винигрет</t>
   </si>
   <si>
-    <t>Свирепая лань</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>F4478-ert</t>
   </si>
   <si>
-    <t>Far478-1207-7850A</t>
-  </si>
-  <si>
     <t>1204-789</t>
   </si>
   <si>
-    <t>ALWE-AP1122-IVORY</t>
-  </si>
-  <si>
     <t>NP100062HJ-147-VORY</t>
   </si>
   <si>
     <t>X-mini</t>
   </si>
   <si>
-    <t>Y-max</t>
-  </si>
-  <si>
-    <t>Free size</t>
-  </si>
-  <si>
     <t>No size</t>
   </si>
   <si>
@@ -131,56 +95,41 @@
     <t>LX</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>2000275733006</t>
-  </si>
-  <si>
-    <t>2000275733008</t>
-  </si>
-  <si>
-    <t>2000275733009</t>
-  </si>
-  <si>
-    <t>2000275733010</t>
-  </si>
-  <si>
-    <t>2000275733011</t>
-  </si>
-  <si>
-    <t>2000275733012</t>
-  </si>
-  <si>
-    <t>2000275733005</t>
-  </si>
-  <si>
     <t>белый</t>
   </si>
   <si>
-    <t>фиолетовы</t>
-  </si>
-  <si>
     <t>буро-малиновы</t>
   </si>
   <si>
-    <t>светло-бежевы</t>
-  </si>
-  <si>
-    <t>светло-сине-коричневы</t>
-  </si>
-  <si>
-    <t>Beige</t>
-  </si>
-  <si>
     <t>BLUE</t>
+  </si>
+  <si>
+    <t>Xart</t>
+  </si>
+  <si>
+    <t>светло-сине-коричневый</t>
+  </si>
+  <si>
+    <t>2000152364126</t>
+  </si>
+  <si>
+    <t>2000080821210</t>
+  </si>
+  <si>
+    <t>2000036947063</t>
+  </si>
+  <si>
+    <t>2000152364119</t>
+  </si>
+  <si>
+    <t>2000152364157</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +147,27 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF4D4D4D"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -207,7 +177,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -215,18 +185,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFE5E5E5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFE5E5E5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFE5E5E5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFE5E5E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -505,201 +499,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2">
+      <c r="E2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="6">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="D3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="6">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>31</v>
+      <c r="D4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>32</v>
+      <c r="D5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="2">
-        <v>48</v>
+      <c r="D6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>35</v>
-      </c>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>